<commit_message>
Change Excel Sheet Name Configuration to remove blank spaces
</commit_message>
<xml_diff>
--- a/VideoGameCatalog.xlsx
+++ b/VideoGameCatalog.xlsx
@@ -9,24 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29016" windowHeight="11580" firstSheet="13" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29016" windowHeight="11580" firstSheet="9" activeTab="14"/>
   </bookViews>
   <sheets>
-    <sheet name="PlayStation 4" sheetId="1" r:id="rId1"/>
-    <sheet name="PlayStation Vita" sheetId="12" r:id="rId2"/>
-    <sheet name="PlayStation 3" sheetId="2" r:id="rId3"/>
-    <sheet name="PlayStation Portable" sheetId="13" r:id="rId4"/>
-    <sheet name="PlayStation 2" sheetId="3" r:id="rId5"/>
+    <sheet name="PlayStation4" sheetId="1" r:id="rId1"/>
+    <sheet name="PlayStationVita" sheetId="12" r:id="rId2"/>
+    <sheet name="PlayStation3" sheetId="2" r:id="rId3"/>
+    <sheet name="PlayStationPortable" sheetId="13" r:id="rId4"/>
+    <sheet name="PlayStation2" sheetId="3" r:id="rId5"/>
     <sheet name="PlayStation" sheetId="4" r:id="rId6"/>
     <sheet name="Xbox" sheetId="5" r:id="rId7"/>
-    <sheet name="Xbox 360" sheetId="6" r:id="rId8"/>
-    <sheet name="Nintendo Wii" sheetId="7" r:id="rId9"/>
-    <sheet name="Nintendo DS" sheetId="8" r:id="rId10"/>
-    <sheet name="Nintendo 3DS" sheetId="9" r:id="rId11"/>
-    <sheet name="Game Boy Color" sheetId="14" r:id="rId12"/>
-    <sheet name="Game Boy Advance" sheetId="15" r:id="rId13"/>
-    <sheet name="Sega Saturn" sheetId="10" r:id="rId14"/>
-    <sheet name="Sega Mega Drive" sheetId="16" r:id="rId15"/>
+    <sheet name="Xbox360" sheetId="6" r:id="rId8"/>
+    <sheet name="NintendoWii" sheetId="7" r:id="rId9"/>
+    <sheet name="NintendoDS" sheetId="8" r:id="rId10"/>
+    <sheet name="Nintendo3DS" sheetId="9" r:id="rId11"/>
+    <sheet name="GameBoyColor" sheetId="14" r:id="rId12"/>
+    <sheet name="GameBoyAdvance" sheetId="15" r:id="rId13"/>
+    <sheet name="SegaSaturn" sheetId="10" r:id="rId14"/>
+    <sheet name="SegaMegaDrive" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -1965,7 +1965,7 @@
   <dimension ref="A1:B178"/>
   <sheetViews>
     <sheetView topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="A178" sqref="A178"/>
+      <selection activeCell="A187" sqref="A187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3400,7 +3400,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3469,7 +3469,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3651,7 +3651,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3753,7 +3753,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3823,7 +3823,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3877,7 +3877,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6796,7 +6796,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6864,7 +6864,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added Methods to Add a New Video Game to an Existing Catalog
</commit_message>
<xml_diff>
--- a/VideoGameCatalog.xlsx
+++ b/VideoGameCatalog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29016" windowHeight="11580" firstSheet="9" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29016" windowHeight="11580" firstSheet="13" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="PlayStation4" sheetId="1" r:id="rId1"/>
@@ -1397,9 +1397,6 @@
     <t>Persona 4</t>
   </si>
   <si>
-    <t>XIII The Video Game</t>
-  </si>
-  <si>
     <t>Capcom Vs SNK 2</t>
   </si>
   <si>
@@ -1512,6 +1509,9 @@
   </si>
   <si>
     <t>Daytona USA</t>
+  </si>
+  <si>
+    <t>Fighting Fury</t>
   </si>
 </sst>
 </file>
@@ -2065,7 +2065,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>17</v>
@@ -2201,7 +2201,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>17</v>
@@ -2249,7 +2249,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>3</v>
@@ -2289,7 +2289,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>17</v>
@@ -2345,7 +2345,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>3</v>
@@ -2361,7 +2361,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>17</v>
@@ -2449,7 +2449,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>17</v>
@@ -2625,7 +2625,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>17</v>
@@ -2873,7 +2873,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>17</v>
@@ -2945,7 +2945,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>17</v>
@@ -3025,7 +3025,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>17</v>
@@ -3305,7 +3305,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>17</v>
@@ -3670,7 +3670,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -3678,7 +3678,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -3686,7 +3686,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -3694,7 +3694,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -3702,7 +3702,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -3710,7 +3710,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -3718,7 +3718,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -3734,7 +3734,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -3772,7 +3772,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -3780,7 +3780,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -3788,7 +3788,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -3796,7 +3796,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -3804,7 +3804,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -3858,7 +3858,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -3896,7 +3896,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
@@ -4111,7 +4111,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B24" t="s">
         <v>17</v>
@@ -4183,7 +4183,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B33" t="s">
         <v>17</v>
@@ -4439,7 +4439,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B65" t="s">
         <v>17</v>
@@ -4631,7 +4631,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B89" t="s">
         <v>17</v>
@@ -5289,7 +5289,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>17</v>
@@ -5473,7 +5473,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>17</v>
@@ -5769,7 +5769,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>17</v>
@@ -5993,7 +5993,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>17</v>
@@ -6121,7 +6121,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B176" s="2" t="s">
         <v>17</v>
@@ -6225,7 +6225,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" s="10" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B189" s="10" t="s">
         <v>3</v>
@@ -6265,7 +6265,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B194" s="2" t="s">
         <v>17</v>
@@ -6497,7 +6497,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>3</v>
@@ -6636,7 +6636,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -6652,7 +6652,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -6724,7 +6724,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>3</v>
@@ -6732,7 +6732,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>445</v>
+        <v>483</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
added Filters to the Excel File
</commit_message>
<xml_diff>
--- a/VideoGameCatalog.xlsx
+++ b/VideoGameCatalog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29016" windowHeight="11580" firstSheet="13" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29016" windowHeight="11580" firstSheet="8" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="PlayStation4" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,23 @@
     <sheet name="SegaSaturn" sheetId="10" r:id="rId14"/>
     <sheet name="SegaMegaDrive" sheetId="16" r:id="rId15"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">GameBoyAdvance!$A$1:$A$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">GameBoyColor!$A$1:$A$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Nintendo3DS!$A$1:$A$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">NintendoDS!$A$1:$A$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">NintendoWii!$A$1:$A$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">PlayStation!$A$1:$A$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">PlayStation2!$A$1:$B$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">PlayStation3!$A$1:$A$226</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PlayStation4!$A$1:$A$176</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">PlayStationPortable!$A$1:$A$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PlayStationVita!$A$1:$A$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">SegaMegaDrive!$A$1:$A$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">SegaSaturn!$A$1:$A$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Xbox!$A$1:$A$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Xbox360!$A$1:$A$2</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1964,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B178"/>
   <sheetViews>
-    <sheetView topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="A187" sqref="A187"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3387,6 +3404,11 @@
       <c r="A178" s="11"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A176">
+    <sortState ref="A2:B176">
+      <sortCondition ref="A1:A176"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:B176">
     <sortCondition ref="A176"/>
   </sortState>
@@ -3400,7 +3422,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3457,6 +3479,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A6">
+    <sortState ref="A2:B6">
+      <sortCondition ref="A1:A6"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:B6">
     <sortCondition ref="A2"/>
   </sortState>
@@ -3469,7 +3496,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3638,6 +3665,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A20">
+    <sortState ref="A2:B20">
+      <sortCondition ref="A1:A20"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:B20">
     <sortCondition ref="A2"/>
   </sortState>
@@ -3651,7 +3683,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3741,6 +3773,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A10">
+    <sortState ref="A2:B10">
+      <sortCondition ref="A1:A10"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:B10">
     <sortCondition ref="A2"/>
   </sortState>
@@ -3753,7 +3790,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3811,6 +3848,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A6">
+    <sortState ref="A2:B6">
+      <sortCondition ref="A1:A6"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:B6">
     <sortCondition ref="A2"/>
   </sortState>
@@ -3823,7 +3865,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3841,30 +3883,35 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A4">
+    <sortState ref="A2:B4">
+      <sortCondition ref="A1:A4"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:B3">
     <sortCondition ref="A2"/>
   </sortState>
@@ -3877,7 +3924,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3907,6 +3954,11 @@
       <c r="B3" s="4"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A3">
+    <sortState ref="A2:B3">
+      <sortCondition ref="A1:A3"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3915,9 +3967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4697,6 +4747,11 @@
       <c r="A100" s="11"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A100">
+    <sortState ref="A2:B100">
+      <sortCondition ref="A1:A100"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:B96">
     <sortCondition ref="A96"/>
   </sortState>
@@ -4709,7 +4764,7 @@
   <dimension ref="A1:B226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6528,6 +6583,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A226">
+    <sortState ref="A2:B226">
+      <sortCondition ref="A1:A226"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:B226">
     <sortCondition ref="A2"/>
   </sortState>
@@ -6540,7 +6600,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6597,6 +6657,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A6">
+    <sortState ref="A2:B6">
+      <sortCondition ref="A1:A6"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:B6">
     <sortCondition ref="A2"/>
   </sortState>
@@ -6606,11 +6671,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6667,16 +6730,16 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>436</v>
+        <v>5</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>3</v>
@@ -6684,31 +6747,31 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>3</v>
@@ -6716,31 +6779,40 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:B15">
+    <sortState ref="A2:B16">
+      <sortCondition ref="A1:A15"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:B15">
-    <sortCondition ref="A15"/>
+    <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6751,7 +6823,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6784,8 +6856,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A3">
+    <sortState ref="A2:B3">
+      <sortCondition ref="A1:A3"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:B3">
-    <sortCondition ref="A2"/>
+    <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6796,7 +6873,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6821,6 +6898,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A2">
+    <sortState ref="A2:B2">
+      <sortCondition ref="A1:A2"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6830,7 +6912,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6855,6 +6937,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A2">
+    <sortState ref="A2:B2">
+      <sortCondition ref="A1:A2"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6864,7 +6951,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6897,6 +6984,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A3">
+    <sortState ref="A2:B3">
+      <sortCondition ref="A1:A3"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>